<commit_message>
corrected plots and pivot tables
</commit_message>
<xml_diff>
--- a/example/param/plot_legend.xlsx
+++ b/example/param/plot_legend.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="60">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -164,7 +164,10 @@
     <t xml:space="preserve">auto_except1_except2</t>
   </si>
   <si>
-    <t xml:space="preserve">auto_col (sur la colonne triée préalablement)</t>
+    <t xml:space="preserve">auto_df_col_minSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colors_col_color1_color2_grades</t>
   </si>
   <si>
     <t xml:space="preserve">list_col1_col2</t>
@@ -173,7 +176,7 @@
     <t xml:space="preserve">col</t>
   </si>
   <si>
-    <t xml:space="preserve">minmax_col_min_max</t>
+    <t xml:space="preserve">minmax_col_minSize_minValue_maxValue</t>
   </si>
   <si>
     <t xml:space="preserve">values_col</t>
@@ -310,30 +313,30 @@
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="40.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="41.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="7.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="6.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="42.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="42.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="7.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,14 +1465,20 @@
   </sheetPr>
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.2734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="45.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="46.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="47.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="42.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,43 +1811,46 @@
       <c r="K7" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="M7" s="0" t="s">
+        <v>48</v>
+      </c>
       <c r="P7" s="0" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N8" s="0" t="s">
         <v>34</v>
@@ -1847,19 +1859,19 @@
         <v>34</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U8" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -1884,10 +1896,10 @@
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>5</v>
@@ -1902,10 +1914,10 @@
         <v>33</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>33</v>
@@ -1967,7 +1979,7 @@
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>